<commit_message>
#71 add example code to second page in spreadsheet
</commit_message>
<xml_diff>
--- a/profile_bluesky/startup/sample_example.xlsx
+++ b/profile_bluesky/startup/sample_example.xlsx
@@ -8,7 +8,8 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sample data" sheetId="1" r:id="rId1"/>
+    <sheet name="demo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Example of Sample positions</t>
   </si>
@@ -33,57 +34,57 @@
     <t>table starts on line 4 (default) with labels, then items</t>
   </si>
   <si>
+    <t>Scan Type</t>
+  </si>
+  <si>
+    <t>sx</t>
+  </si>
+  <si>
+    <t>sy</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>USAXSscan</t>
+  </si>
+  <si>
+    <t>Water Blank</t>
+  </si>
+  <si>
+    <t>saxsExp</t>
+  </si>
+  <si>
+    <t>waxwsExp</t>
+  </si>
+  <si>
+    <t>plastic</t>
+  </si>
+  <si>
+    <t>Al foil</t>
+  </si>
+  <si>
     <t>example code:</t>
   </si>
   <si>
-    <t>Scan Type</t>
-  </si>
-  <si>
-    <t>sx</t>
-  </si>
-  <si>
-    <t>sy</t>
-  </si>
-  <si>
-    <t>Thickness</t>
-  </si>
-  <si>
-    <t>Sample Name</t>
-  </si>
-  <si>
     <t>import APS_BlueSky_tools.utils as APS_utils</t>
   </si>
   <si>
-    <t>USAXSscan</t>
-  </si>
-  <si>
-    <t>Water Blank</t>
-  </si>
-  <si>
     <t>excel_file = os.path.abspath("./sample_example.xlsx")</t>
   </si>
   <si>
-    <t>saxsExp</t>
-  </si>
-  <si>
     <t>excel = APS_utils.ExcelDatabaseFileGeneric(excel_file)</t>
   </si>
   <si>
-    <t>waxwsExp</t>
-  </si>
-  <si>
     <t>for scan in excel.db.values():</t>
   </si>
   <si>
-    <t>plastic</t>
-  </si>
-  <si>
     <t xml:space="preserve">    print(scan)</t>
   </si>
   <si>
-    <t>Al foil</t>
-  </si>
-  <si>
     <t>prints out:</t>
   </si>
   <si>
@@ -100,13 +101,19 @@
   </si>
   <si>
     <t>{'Scan Type': 'USAXSscan', 'sx': 12, 'sy': 37, 'Thickness': 0.1, 'Sample Name': 'Al foil'}</t>
+  </si>
+  <si>
+    <t>this command:</t>
+  </si>
+  <si>
+    <t>print(excel.db["3"]["Sample Name"])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +131,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Courier New"/>
@@ -149,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +177,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,10 +518,9 @@
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25">
+    <row r="1" spans="1:5" ht="23.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -510,7 +529,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -519,37 +538,31 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>8</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>10</v>
       </c>
       <c r="B5">
         <v>45.07</v>
@@ -561,15 +574,12 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>45.07</v>
@@ -581,15 +591,12 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>11</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>15</v>
       </c>
       <c r="B7">
         <v>45.07</v>
@@ -601,15 +608,12 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -621,15 +625,12 @@
         <v>1.2</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -641,51 +642,8 @@
         <v>0.1</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="I10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="I11" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="I12" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="I13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="I14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="I15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="9:9">
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="9:9">
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="9:9">
-      <c r="I19" s="4"/>
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -696,4 +654,100 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E47752-DDFC-4A61-AEC7-8FEA20C684E3}">
+  <dimension ref="A3:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" xr3:uid="{F73A3E4B-8674-5DD4-9069-E656CB63158B}">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75">
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75">
+      <c r="B13" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75">
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75">
+      <c r="B15" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75">
+      <c r="B16" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75">
+      <c r="B20" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>